<commit_message>
EPBDS-7063 change constructor priority
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7063.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7063.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\opHome2\user-workspace\admin\EPBDS-7063\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\git-openl\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEF9275-161F-4010-ABD4-4054AC2B3617}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CCB9D8-0BD6-40EC-B85D-8DCB6B9D0123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB10D87C-C96D-43F2-BCAD-D1117D91297B}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="50">
   <si>
     <t>String</t>
   </si>
@@ -90,15 +90,6 @@
     <t>step3</t>
   </si>
   <si>
-    <t>string2</t>
-  </si>
-  <si>
-    <t>String2</t>
-  </si>
-  <si>
-    <t>=Date(month=14);</t>
-  </si>
-  <si>
     <t>Datatype type1</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
     <t>defaultStringValue2</t>
   </si>
   <si>
-    <t>Test mySpr spr1Test</t>
-  </si>
-  <si>
     <t>type2</t>
   </si>
   <si>
@@ -123,102 +111,80 @@
     <t>Spreadsheet Date datesSpr(String string, Integer numParam)</t>
   </si>
   <si>
-    <t>Spreadsheet type1 spr2(String stringParam, Integer numParam)</t>
-  </si>
-  <si>
-    <t>=type1(str2=stringParam, num1=2, num3=numParam, type2 = type2(str1="newValue", num3 = numParam));</t>
-  </si>
-  <si>
     <t>Datatype type3</t>
   </si>
   <si>
     <t>type3</t>
   </si>
   <si>
-    <t>=type1(num3=numParam, type2 = type2(num3 = numParam, type3=type3(num3 = numParam)));</t>
-  </si>
-  <si>
-    <t>Test mySpr2 spr2Test</t>
-  </si>
-  <si>
-    <t>Test mySpr3 spr3Test</t>
-  </si>
-  <si>
-    <t>Spreadsheet type1 spr3(String stringParam, Integer numParam)</t>
-  </si>
-  <si>
     <t>Test spr1 spr1Test</t>
   </si>
   <si>
     <t>stringParam</t>
   </si>
   <si>
-    <t>String2stringParam</t>
-  </si>
-  <si>
     <t>Test spr2 spr2Test</t>
   </si>
   <si>
+    <t>_res_.type2.num3</t>
+  </si>
+  <si>
+    <t>type2num3</t>
+  </si>
+  <si>
+    <t>=Date(2021,04,08);</t>
+  </si>
+  <si>
+    <t>Spreadsheet type1 spr3(String stringParam, Integer num3)</t>
+  </si>
+  <si>
+    <t>=type1(num3=num3, type2 = type2(num3 = num3, type3=type3(num3 = num3)));</t>
+  </si>
+  <si>
+    <t>Spreadsheet type1 spr2(String stringParam, Integer numParam1, Double numParam2)</t>
+  </si>
+  <si>
+    <t>=type1(str2=stringParam, num1=2, num3=numParam1, type2 = type2(str1="newValue", num3 = numParam2));</t>
+  </si>
+  <si>
+    <t>numParam2</t>
+  </si>
+  <si>
+    <t>numParam1</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>=type2(str2=stringParam, num3=numParam1, type3 = type3(numParam2));</t>
+  </si>
+  <si>
+    <t>Test spr4 spr4Test</t>
+  </si>
+  <si>
+    <t>Spreadsheet type2 spr4(String stringParam, Integer numParam1, Double numParam2)</t>
+  </si>
+  <si>
+    <t>_res_.type3.num3</t>
+  </si>
+  <si>
     <t>Test spr3 spr3Test</t>
   </si>
   <si>
-    <t>_res_.type2.num3</t>
-  </si>
-  <si>
-    <t>type2num3</t>
-  </si>
-  <si>
-    <t>_res_.type2.typ3.num3</t>
+    <t>_res_.type2.type3.num3</t>
   </si>
   <si>
     <t>type2type3num3</t>
-  </si>
-  <si>
-    <t>_res_.type2.type3.num3</t>
-  </si>
-  <si>
-    <t>=Date(2021,04,08);</t>
-  </si>
-  <si>
-    <t>Spreadsheet type1 spr3(String stringParam, Integer num3)</t>
-  </si>
-  <si>
-    <t>=type1(num3=numParam, type2 = type2(num3 = numParam, type3=type3(num3 = num3)));</t>
-  </si>
-  <si>
-    <t>=type1(num3=num3, type2 = type2(num3 = num3, type3=type3(num3 = num3)));</t>
-  </si>
-  <si>
-    <t>Spreadsheet type1 spr2(String stringParam, Integer numParam1, Integer numParam2)</t>
-  </si>
-  <si>
-    <t>Spreadsheet type1 spr2(String stringParam, Integer numParam1, Double numParam2)</t>
-  </si>
-  <si>
-    <t>=type1(str2=stringParam, num1=2, num3=numParam1, type2 = type2(str1="newValue", num3 = numParam2));</t>
-  </si>
-  <si>
-    <t>numParam2</t>
-  </si>
-  <si>
-    <t>numParam1</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>3.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -287,28 +253,62 @@
       <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <right style="thin"/>
-      <top style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -317,14 +317,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -639,28 +649,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAACCCC-E093-418B-9263-C47311F78D95}">
-  <dimension ref="B4:L40"/>
+  <dimension ref="B4:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.21875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="21.44140625" collapsed="true"/>
+    <col min="3" max="3" width="91.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -678,7 +688,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
         <v>1</v>
@@ -712,7 +722,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
         <v>0</v>
@@ -732,15 +742,15 @@
       <c r="L9" s="5"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="10"/>
+      <c r="B10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="14"/>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L10" s="5"/>
     </row>
@@ -757,21 +767,19 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="B14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="14"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="J14" t="s">
@@ -788,8 +796,6 @@
       <c r="C15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="J15" t="s">
@@ -799,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
@@ -807,10 +813,8 @@
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+        <v>37</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="J16" t="s">
@@ -822,37 +826,41 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="B19" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>20</v>
+      <c r="B21" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
       <c r="J21" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -867,301 +875,387 @@
       <c r="L22" s="7"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
       <c r="L24" s="7"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>14</v>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C30" s="2">
         <v>33</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F30" s="3">
         <v>2</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G30" s="3">
         <v>222</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H30" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="11"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="6" t="s">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="6" t="s">
+      <c r="D34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I34" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J32" t="s" s="6">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="6" t="s">
+      <c r="J34" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="D35" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I35" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J33" t="s" s="6">
+      <c r="J35" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="6">
+        <v>33</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="3">
+        <v>2</v>
+      </c>
+      <c r="H36" s="3">
+        <v>222</v>
+      </c>
+      <c r="I36" s="3">
+        <v>33</v>
+      </c>
+      <c r="J36" s="3">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="11">
+        <v>33</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="19">
+        <v>2</v>
+      </c>
+      <c r="G41" s="19">
+        <v>222</v>
+      </c>
+      <c r="H41" s="19">
+        <v>33</v>
+      </c>
+      <c r="I41" s="19">
+        <v>33</v>
+      </c>
+      <c r="J41" s="19">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C46" s="9">
         <v>33</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="3" t="s">
+      <c r="D46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H34" s="3" t="n">
-        <v>222.0</v>
-      </c>
-      <c r="I34" t="n" s="3">
-        <v>33.0</v>
-      </c>
-      <c r="J34" t="n" s="3">
+      <c r="F46" s="3">
         <v>3.4</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="6">
-        <v>33</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="3">
-        <v>2</v>
-      </c>
-      <c r="G40" s="3">
-        <v>222</v>
-      </c>
-      <c r="H40" s="3" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="I40" s="3" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="J40" t="n" s="3">
-        <v>33.0</v>
-      </c>
-    </row>
+    <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B19:C19"/>
+  <mergeCells count="8">
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B38:J38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>